<commit_message>
fixing python script and updating requirements
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -138,10 +138,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T72"/>
+  <dimension ref="A1:X72"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
+      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -159,7 +159,27 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0"/>
+      <c r="E1" s="0"/>
+      <c r="F1" s="0"/>
+      <c r="G1" s="0"/>
+      <c r="H1" s="0"/>
+      <c r="I1" s="0"/>
+      <c r="J1" s="0"/>
+      <c r="K1" s="0"/>
+      <c r="L1" s="0"/>
+      <c r="M1" s="0"/>
+      <c r="N1" s="0"/>
+      <c r="O1" s="0"/>
+      <c r="P1" s="0"/>
+      <c r="Q1" s="0"/>
+      <c r="R1" s="0"/>
+      <c r="S1" s="0"/>
       <c r="T1" s="0"/>
+      <c r="U1" s="0"/>
+      <c r="V1" s="0"/>
+      <c r="W1" s="0"/>
+      <c r="X1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
@@ -171,18 +191,27 @@
       <c r="C2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="S2" s="3"/>
+      <c r="D2" s="0"/>
+      <c r="E2" s="0"/>
+      <c r="F2" s="0"/>
+      <c r="G2" s="0"/>
+      <c r="H2" s="0"/>
+      <c r="I2" s="0"/>
+      <c r="J2" s="0"/>
+      <c r="K2" s="0"/>
+      <c r="L2" s="0"/>
+      <c r="M2" s="0"/>
+      <c r="N2" s="0"/>
+      <c r="O2" s="0"/>
+      <c r="P2" s="0"/>
+      <c r="Q2" s="0"/>
+      <c r="R2" s="0"/>
+      <c r="S2" s="0"/>
       <c r="T2" s="0"/>
+      <c r="U2" s="0"/>
+      <c r="V2" s="0"/>
+      <c r="W2" s="0"/>
+      <c r="X2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
@@ -194,18 +223,27 @@
       <c r="C3" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="S3" s="3"/>
+      <c r="D3" s="0"/>
+      <c r="E3" s="0"/>
+      <c r="F3" s="0"/>
+      <c r="G3" s="0"/>
+      <c r="H3" s="0"/>
+      <c r="I3" s="0"/>
+      <c r="J3" s="0"/>
+      <c r="K3" s="0"/>
+      <c r="L3" s="0"/>
+      <c r="M3" s="0"/>
+      <c r="N3" s="0"/>
+      <c r="O3" s="0"/>
+      <c r="P3" s="0"/>
+      <c r="Q3" s="0"/>
+      <c r="R3" s="0"/>
+      <c r="S3" s="0"/>
       <c r="T3" s="0"/>
+      <c r="U3" s="0"/>
+      <c r="V3" s="0"/>
+      <c r="W3" s="0"/>
+      <c r="X3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -217,18 +255,27 @@
       <c r="C4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="S4" s="3"/>
+      <c r="D4" s="0"/>
+      <c r="E4" s="0"/>
+      <c r="F4" s="0"/>
+      <c r="G4" s="0"/>
+      <c r="H4" s="0"/>
+      <c r="I4" s="0"/>
+      <c r="J4" s="0"/>
+      <c r="K4" s="0"/>
+      <c r="L4" s="0"/>
+      <c r="M4" s="0"/>
+      <c r="N4" s="0"/>
+      <c r="O4" s="0"/>
+      <c r="P4" s="0"/>
+      <c r="Q4" s="0"/>
+      <c r="R4" s="0"/>
+      <c r="S4" s="0"/>
       <c r="T4" s="0"/>
+      <c r="U4" s="0"/>
+      <c r="V4" s="0"/>
+      <c r="W4" s="0"/>
+      <c r="X4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -240,18 +287,27 @@
       <c r="C5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="S5" s="3"/>
+      <c r="D5" s="0"/>
+      <c r="E5" s="0"/>
+      <c r="F5" s="0"/>
+      <c r="G5" s="0"/>
+      <c r="H5" s="0"/>
+      <c r="I5" s="0"/>
+      <c r="J5" s="0"/>
+      <c r="K5" s="0"/>
+      <c r="L5" s="0"/>
+      <c r="M5" s="0"/>
+      <c r="N5" s="0"/>
+      <c r="O5" s="0"/>
+      <c r="P5" s="0"/>
+      <c r="Q5" s="0"/>
+      <c r="R5" s="0"/>
+      <c r="S5" s="0"/>
       <c r="T5" s="0"/>
+      <c r="U5" s="0"/>
+      <c r="V5" s="0"/>
+      <c r="W5" s="0"/>
+      <c r="X5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -263,15 +319,27 @@
       <c r="C6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="S6" s="3"/>
+      <c r="D6" s="0"/>
+      <c r="E6" s="0"/>
+      <c r="F6" s="0"/>
+      <c r="G6" s="0"/>
+      <c r="H6" s="0"/>
+      <c r="I6" s="0"/>
+      <c r="J6" s="0"/>
+      <c r="K6" s="0"/>
+      <c r="L6" s="0"/>
+      <c r="M6" s="0"/>
+      <c r="N6" s="0"/>
+      <c r="O6" s="0"/>
+      <c r="P6" s="0"/>
+      <c r="Q6" s="0"/>
+      <c r="R6" s="0"/>
+      <c r="S6" s="0"/>
       <c r="T6" s="0"/>
+      <c r="U6" s="0"/>
+      <c r="V6" s="0"/>
+      <c r="W6" s="0"/>
+      <c r="X6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
@@ -283,17 +351,27 @@
       <c r="C7" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="S7" s="3"/>
+      <c r="D7" s="0"/>
+      <c r="E7" s="0"/>
+      <c r="F7" s="0"/>
+      <c r="G7" s="0"/>
+      <c r="H7" s="0"/>
+      <c r="I7" s="0"/>
+      <c r="J7" s="0"/>
+      <c r="K7" s="0"/>
+      <c r="L7" s="0"/>
+      <c r="M7" s="0"/>
+      <c r="N7" s="0"/>
+      <c r="O7" s="0"/>
+      <c r="P7" s="0"/>
+      <c r="Q7" s="0"/>
+      <c r="R7" s="0"/>
+      <c r="S7" s="0"/>
       <c r="T7" s="0"/>
+      <c r="U7" s="0"/>
+      <c r="V7" s="0"/>
+      <c r="W7" s="0"/>
+      <c r="X7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
@@ -305,17 +383,27 @@
       <c r="C8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="S8" s="3"/>
+      <c r="D8" s="0"/>
+      <c r="E8" s="0"/>
+      <c r="F8" s="0"/>
+      <c r="G8" s="0"/>
+      <c r="H8" s="0"/>
+      <c r="I8" s="0"/>
+      <c r="J8" s="0"/>
+      <c r="K8" s="0"/>
+      <c r="L8" s="0"/>
+      <c r="M8" s="0"/>
+      <c r="N8" s="0"/>
+      <c r="O8" s="0"/>
+      <c r="P8" s="0"/>
+      <c r="Q8" s="0"/>
+      <c r="R8" s="0"/>
+      <c r="S8" s="0"/>
       <c r="T8" s="0"/>
+      <c r="U8" s="0"/>
+      <c r="V8" s="0"/>
+      <c r="W8" s="0"/>
+      <c r="X8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -327,16 +415,27 @@
       <c r="C9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="S9" s="3"/>
+      <c r="D9" s="0"/>
+      <c r="E9" s="0"/>
+      <c r="F9" s="0"/>
+      <c r="G9" s="0"/>
+      <c r="H9" s="0"/>
+      <c r="I9" s="0"/>
+      <c r="J9" s="0"/>
+      <c r="K9" s="0"/>
+      <c r="L9" s="0"/>
+      <c r="M9" s="0"/>
+      <c r="N9" s="0"/>
+      <c r="O9" s="0"/>
+      <c r="P9" s="0"/>
+      <c r="Q9" s="0"/>
+      <c r="R9" s="0"/>
+      <c r="S9" s="0"/>
       <c r="T9" s="0"/>
+      <c r="U9" s="0"/>
+      <c r="V9" s="0"/>
+      <c r="W9" s="0"/>
+      <c r="X9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
@@ -348,15 +447,27 @@
       <c r="C10" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="S10" s="3"/>
+      <c r="D10" s="0"/>
+      <c r="E10" s="0"/>
+      <c r="F10" s="0"/>
+      <c r="G10" s="0"/>
+      <c r="H10" s="0"/>
+      <c r="I10" s="0"/>
+      <c r="J10" s="0"/>
+      <c r="K10" s="0"/>
+      <c r="L10" s="0"/>
+      <c r="M10" s="0"/>
+      <c r="N10" s="0"/>
+      <c r="O10" s="0"/>
+      <c r="P10" s="0"/>
+      <c r="Q10" s="0"/>
+      <c r="R10" s="0"/>
+      <c r="S10" s="0"/>
       <c r="T10" s="0"/>
+      <c r="U10" s="0"/>
+      <c r="V10" s="0"/>
+      <c r="W10" s="0"/>
+      <c r="X10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -368,15 +479,27 @@
       <c r="C11" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="S11" s="3"/>
+      <c r="D11" s="0"/>
+      <c r="E11" s="0"/>
+      <c r="F11" s="0"/>
+      <c r="G11" s="0"/>
+      <c r="H11" s="0"/>
+      <c r="I11" s="0"/>
+      <c r="J11" s="0"/>
+      <c r="K11" s="0"/>
+      <c r="L11" s="0"/>
+      <c r="M11" s="0"/>
+      <c r="N11" s="0"/>
+      <c r="O11" s="0"/>
+      <c r="P11" s="0"/>
+      <c r="Q11" s="0"/>
+      <c r="R11" s="0"/>
+      <c r="S11" s="0"/>
       <c r="T11" s="0"/>
+      <c r="U11" s="0"/>
+      <c r="V11" s="0"/>
+      <c r="W11" s="0"/>
+      <c r="X11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
@@ -388,15 +511,27 @@
       <c r="C12" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="R12" s="3"/>
+      <c r="D12" s="0"/>
+      <c r="E12" s="0"/>
+      <c r="F12" s="0"/>
+      <c r="G12" s="0"/>
+      <c r="H12" s="0"/>
+      <c r="I12" s="0"/>
+      <c r="J12" s="0"/>
+      <c r="K12" s="0"/>
+      <c r="L12" s="0"/>
+      <c r="M12" s="0"/>
+      <c r="N12" s="0"/>
+      <c r="O12" s="0"/>
+      <c r="P12" s="0"/>
+      <c r="Q12" s="0"/>
+      <c r="R12" s="0"/>
+      <c r="S12" s="0"/>
       <c r="T12" s="0"/>
+      <c r="U12" s="0"/>
+      <c r="V12" s="0"/>
+      <c r="W12" s="0"/>
+      <c r="X12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
@@ -408,15 +543,27 @@
       <c r="C13" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="R13" s="3"/>
+      <c r="D13" s="0"/>
+      <c r="E13" s="0"/>
+      <c r="F13" s="0"/>
+      <c r="G13" s="0"/>
+      <c r="H13" s="0"/>
+      <c r="I13" s="0"/>
+      <c r="J13" s="0"/>
+      <c r="K13" s="0"/>
+      <c r="L13" s="0"/>
+      <c r="M13" s="0"/>
+      <c r="N13" s="0"/>
+      <c r="O13" s="0"/>
+      <c r="P13" s="0"/>
+      <c r="Q13" s="0"/>
+      <c r="R13" s="0"/>
+      <c r="S13" s="0"/>
       <c r="T13" s="0"/>
+      <c r="U13" s="0"/>
+      <c r="V13" s="0"/>
+      <c r="W13" s="0"/>
+      <c r="X13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
@@ -428,16 +575,27 @@
       <c r="C14" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="R14" s="3"/>
+      <c r="D14" s="0"/>
+      <c r="E14" s="0"/>
+      <c r="F14" s="0"/>
+      <c r="G14" s="0"/>
+      <c r="H14" s="0"/>
+      <c r="I14" s="0"/>
+      <c r="J14" s="0"/>
+      <c r="K14" s="0"/>
+      <c r="L14" s="0"/>
+      <c r="M14" s="0"/>
+      <c r="N14" s="0"/>
+      <c r="O14" s="0"/>
+      <c r="P14" s="0"/>
+      <c r="Q14" s="0"/>
+      <c r="R14" s="0"/>
+      <c r="S14" s="0"/>
       <c r="T14" s="0"/>
+      <c r="U14" s="0"/>
+      <c r="V14" s="0"/>
+      <c r="W14" s="0"/>
+      <c r="X14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
@@ -449,16 +607,27 @@
       <c r="C15" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="R15" s="3"/>
+      <c r="D15" s="0"/>
+      <c r="E15" s="0"/>
+      <c r="F15" s="0"/>
+      <c r="G15" s="0"/>
+      <c r="H15" s="0"/>
+      <c r="I15" s="0"/>
+      <c r="J15" s="0"/>
+      <c r="K15" s="0"/>
+      <c r="L15" s="0"/>
+      <c r="M15" s="0"/>
+      <c r="N15" s="0"/>
+      <c r="O15" s="0"/>
+      <c r="P15" s="0"/>
+      <c r="Q15" s="0"/>
+      <c r="R15" s="0"/>
+      <c r="S15" s="0"/>
       <c r="T15" s="0"/>
+      <c r="U15" s="0"/>
+      <c r="V15" s="0"/>
+      <c r="W15" s="0"/>
+      <c r="X15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
@@ -470,14 +639,27 @@
       <c r="C16" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="R16" s="3"/>
+      <c r="D16" s="0"/>
+      <c r="E16" s="0"/>
+      <c r="F16" s="0"/>
+      <c r="G16" s="0"/>
+      <c r="H16" s="0"/>
+      <c r="I16" s="0"/>
+      <c r="J16" s="0"/>
+      <c r="K16" s="0"/>
+      <c r="L16" s="0"/>
+      <c r="M16" s="0"/>
+      <c r="N16" s="0"/>
+      <c r="O16" s="0"/>
+      <c r="P16" s="0"/>
+      <c r="Q16" s="0"/>
+      <c r="R16" s="0"/>
+      <c r="S16" s="0"/>
       <c r="T16" s="0"/>
+      <c r="U16" s="0"/>
+      <c r="V16" s="0"/>
+      <c r="W16" s="0"/>
+      <c r="X16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
@@ -489,16 +671,27 @@
       <c r="C17" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="R17" s="3"/>
-      <c r="S17" s="3"/>
+      <c r="D17" s="0"/>
+      <c r="E17" s="0"/>
+      <c r="F17" s="0"/>
+      <c r="G17" s="0"/>
+      <c r="H17" s="0"/>
+      <c r="I17" s="0"/>
+      <c r="J17" s="0"/>
+      <c r="K17" s="0"/>
+      <c r="L17" s="0"/>
+      <c r="M17" s="0"/>
+      <c r="N17" s="0"/>
+      <c r="O17" s="0"/>
+      <c r="P17" s="0"/>
+      <c r="Q17" s="0"/>
+      <c r="R17" s="0"/>
+      <c r="S17" s="0"/>
       <c r="T17" s="0"/>
+      <c r="U17" s="0"/>
+      <c r="V17" s="0"/>
+      <c r="W17" s="0"/>
+      <c r="X17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
@@ -510,18 +703,27 @@
       <c r="C18" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
+      <c r="D18" s="0"/>
+      <c r="E18" s="0"/>
+      <c r="F18" s="0"/>
+      <c r="G18" s="0"/>
+      <c r="H18" s="0"/>
+      <c r="I18" s="0"/>
+      <c r="J18" s="0"/>
+      <c r="K18" s="0"/>
+      <c r="L18" s="0"/>
+      <c r="M18" s="0"/>
+      <c r="N18" s="0"/>
+      <c r="O18" s="0"/>
+      <c r="P18" s="0"/>
+      <c r="Q18" s="0"/>
+      <c r="R18" s="0"/>
+      <c r="S18" s="0"/>
       <c r="T18" s="0"/>
+      <c r="U18" s="0"/>
+      <c r="V18" s="0"/>
+      <c r="W18" s="0"/>
+      <c r="X18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
@@ -533,18 +735,27 @@
       <c r="C19" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
+      <c r="D19" s="0"/>
+      <c r="E19" s="0"/>
+      <c r="F19" s="0"/>
+      <c r="G19" s="0"/>
+      <c r="H19" s="0"/>
+      <c r="I19" s="0"/>
+      <c r="J19" s="0"/>
+      <c r="K19" s="0"/>
+      <c r="L19" s="0"/>
+      <c r="M19" s="0"/>
+      <c r="N19" s="0"/>
+      <c r="O19" s="0"/>
+      <c r="P19" s="0"/>
+      <c r="Q19" s="0"/>
+      <c r="R19" s="0"/>
+      <c r="S19" s="0"/>
       <c r="T19" s="0"/>
+      <c r="U19" s="0"/>
+      <c r="V19" s="0"/>
+      <c r="W19" s="0"/>
+      <c r="X19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
@@ -556,18 +767,27 @@
       <c r="C20" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
+      <c r="D20" s="0"/>
+      <c r="E20" s="0"/>
+      <c r="F20" s="0"/>
+      <c r="G20" s="0"/>
+      <c r="H20" s="0"/>
+      <c r="I20" s="0"/>
+      <c r="J20" s="0"/>
+      <c r="K20" s="0"/>
+      <c r="L20" s="0"/>
+      <c r="M20" s="0"/>
+      <c r="N20" s="0"/>
+      <c r="O20" s="0"/>
+      <c r="P20" s="0"/>
+      <c r="Q20" s="0"/>
+      <c r="R20" s="0"/>
+      <c r="S20" s="0"/>
       <c r="T20" s="0"/>
+      <c r="U20" s="0"/>
+      <c r="V20" s="0"/>
+      <c r="W20" s="0"/>
+      <c r="X20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
@@ -579,15 +799,27 @@
       <c r="C21" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
+      <c r="D21" s="0"/>
+      <c r="E21" s="0"/>
+      <c r="F21" s="0"/>
+      <c r="G21" s="0"/>
+      <c r="H21" s="0"/>
+      <c r="I21" s="0"/>
+      <c r="J21" s="0"/>
+      <c r="K21" s="0"/>
+      <c r="L21" s="0"/>
+      <c r="M21" s="0"/>
+      <c r="N21" s="0"/>
+      <c r="O21" s="0"/>
+      <c r="P21" s="0"/>
+      <c r="Q21" s="0"/>
+      <c r="R21" s="0"/>
+      <c r="S21" s="0"/>
       <c r="T21" s="0"/>
+      <c r="U21" s="0"/>
+      <c r="V21" s="0"/>
+      <c r="W21" s="0"/>
+      <c r="X21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
@@ -599,14 +831,27 @@
       <c r="C22" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="R22" s="3"/>
+      <c r="D22" s="0"/>
+      <c r="E22" s="0"/>
+      <c r="F22" s="0"/>
+      <c r="G22" s="0"/>
+      <c r="H22" s="0"/>
+      <c r="I22" s="0"/>
+      <c r="J22" s="0"/>
+      <c r="K22" s="0"/>
+      <c r="L22" s="0"/>
+      <c r="M22" s="0"/>
+      <c r="N22" s="0"/>
+      <c r="O22" s="0"/>
+      <c r="P22" s="0"/>
+      <c r="Q22" s="0"/>
+      <c r="R22" s="0"/>
+      <c r="S22" s="0"/>
       <c r="T22" s="0"/>
+      <c r="U22" s="0"/>
+      <c r="V22" s="0"/>
+      <c r="W22" s="0"/>
+      <c r="X22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
@@ -618,16 +863,27 @@
       <c r="C23" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="R23" s="3"/>
+      <c r="D23" s="0"/>
+      <c r="E23" s="0"/>
+      <c r="F23" s="0"/>
+      <c r="G23" s="0"/>
+      <c r="H23" s="0"/>
+      <c r="I23" s="0"/>
+      <c r="J23" s="0"/>
+      <c r="K23" s="0"/>
+      <c r="L23" s="0"/>
+      <c r="M23" s="0"/>
+      <c r="N23" s="0"/>
+      <c r="O23" s="0"/>
+      <c r="P23" s="0"/>
+      <c r="Q23" s="0"/>
+      <c r="R23" s="0"/>
+      <c r="S23" s="0"/>
       <c r="T23" s="0"/>
+      <c r="U23" s="0"/>
+      <c r="V23" s="0"/>
+      <c r="W23" s="0"/>
+      <c r="X23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
@@ -639,16 +895,27 @@
       <c r="C24" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="R24" s="3"/>
+      <c r="D24" s="0"/>
+      <c r="E24" s="0"/>
+      <c r="F24" s="0"/>
+      <c r="G24" s="0"/>
+      <c r="H24" s="0"/>
+      <c r="I24" s="0"/>
+      <c r="J24" s="0"/>
+      <c r="K24" s="0"/>
+      <c r="L24" s="0"/>
+      <c r="M24" s="0"/>
+      <c r="N24" s="0"/>
+      <c r="O24" s="0"/>
+      <c r="P24" s="0"/>
+      <c r="Q24" s="0"/>
+      <c r="R24" s="0"/>
+      <c r="S24" s="0"/>
       <c r="T24" s="0"/>
+      <c r="U24" s="0"/>
+      <c r="V24" s="0"/>
+      <c r="W24" s="0"/>
+      <c r="X24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
@@ -660,17 +927,27 @@
       <c r="C25" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
-      <c r="R25" s="3"/>
-      <c r="S25" s="3"/>
+      <c r="D25" s="0"/>
+      <c r="E25" s="0"/>
+      <c r="F25" s="0"/>
+      <c r="G25" s="0"/>
+      <c r="H25" s="0"/>
+      <c r="I25" s="0"/>
+      <c r="J25" s="0"/>
+      <c r="K25" s="0"/>
+      <c r="L25" s="0"/>
+      <c r="M25" s="0"/>
+      <c r="N25" s="0"/>
+      <c r="O25" s="0"/>
+      <c r="P25" s="0"/>
+      <c r="Q25" s="0"/>
+      <c r="R25" s="0"/>
+      <c r="S25" s="0"/>
       <c r="T25" s="0"/>
+      <c r="U25" s="0"/>
+      <c r="V25" s="0"/>
+      <c r="W25" s="0"/>
+      <c r="X25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
@@ -682,17 +959,27 @@
       <c r="C26" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
-      <c r="R26" s="3"/>
-      <c r="S26" s="3"/>
+      <c r="D26" s="0"/>
+      <c r="E26" s="0"/>
+      <c r="F26" s="0"/>
+      <c r="G26" s="0"/>
+      <c r="H26" s="0"/>
+      <c r="I26" s="0"/>
+      <c r="J26" s="0"/>
+      <c r="K26" s="0"/>
+      <c r="L26" s="0"/>
+      <c r="M26" s="0"/>
+      <c r="N26" s="0"/>
+      <c r="O26" s="0"/>
+      <c r="P26" s="0"/>
+      <c r="Q26" s="0"/>
+      <c r="R26" s="0"/>
+      <c r="S26" s="0"/>
       <c r="T26" s="0"/>
+      <c r="U26" s="0"/>
+      <c r="V26" s="0"/>
+      <c r="W26" s="0"/>
+      <c r="X26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
@@ -704,15 +991,27 @@
       <c r="C27" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="O27" s="3"/>
-      <c r="R27" s="3"/>
-      <c r="S27" s="3"/>
+      <c r="D27" s="0"/>
+      <c r="E27" s="0"/>
+      <c r="F27" s="0"/>
+      <c r="G27" s="0"/>
+      <c r="H27" s="0"/>
+      <c r="I27" s="0"/>
+      <c r="J27" s="0"/>
+      <c r="K27" s="0"/>
+      <c r="L27" s="0"/>
+      <c r="M27" s="0"/>
+      <c r="N27" s="0"/>
+      <c r="O27" s="0"/>
+      <c r="P27" s="0"/>
+      <c r="Q27" s="0"/>
+      <c r="R27" s="0"/>
+      <c r="S27" s="0"/>
       <c r="T27" s="0"/>
+      <c r="U27" s="0"/>
+      <c r="V27" s="0"/>
+      <c r="W27" s="0"/>
+      <c r="X27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
@@ -724,13 +1023,27 @@
       <c r="C28" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="P28" s="3"/>
-      <c r="R28" s="3"/>
-      <c r="S28" s="3"/>
+      <c r="D28" s="0"/>
+      <c r="E28" s="0"/>
+      <c r="F28" s="0"/>
+      <c r="G28" s="0"/>
+      <c r="H28" s="0"/>
+      <c r="I28" s="0"/>
+      <c r="J28" s="0"/>
+      <c r="K28" s="0"/>
+      <c r="L28" s="0"/>
+      <c r="M28" s="0"/>
+      <c r="N28" s="0"/>
+      <c r="O28" s="0"/>
+      <c r="P28" s="0"/>
+      <c r="Q28" s="0"/>
+      <c r="R28" s="0"/>
+      <c r="S28" s="0"/>
       <c r="T28" s="0"/>
+      <c r="U28" s="0"/>
+      <c r="V28" s="0"/>
+      <c r="W28" s="0"/>
+      <c r="X28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
@@ -742,10 +1055,27 @@
       <c r="C29" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F29" s="3"/>
-      <c r="P29" s="3"/>
-      <c r="R29" s="3"/>
+      <c r="D29" s="0"/>
+      <c r="E29" s="0"/>
+      <c r="F29" s="0"/>
+      <c r="G29" s="0"/>
+      <c r="H29" s="0"/>
+      <c r="I29" s="0"/>
+      <c r="J29" s="0"/>
+      <c r="K29" s="0"/>
+      <c r="L29" s="0"/>
+      <c r="M29" s="0"/>
+      <c r="N29" s="0"/>
+      <c r="O29" s="0"/>
+      <c r="P29" s="0"/>
+      <c r="Q29" s="0"/>
+      <c r="R29" s="0"/>
+      <c r="S29" s="0"/>
       <c r="T29" s="0"/>
+      <c r="U29" s="0"/>
+      <c r="V29" s="0"/>
+      <c r="W29" s="0"/>
+      <c r="X29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
@@ -757,60 +1087,123 @@
       <c r="C30" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="P30" s="3"/>
-      <c r="R30" s="3"/>
+      <c r="D30" s="0"/>
+      <c r="E30" s="0"/>
+      <c r="F30" s="0"/>
+      <c r="G30" s="0"/>
+      <c r="H30" s="0"/>
+      <c r="I30" s="0"/>
+      <c r="J30" s="0"/>
+      <c r="K30" s="0"/>
+      <c r="L30" s="0"/>
+      <c r="M30" s="0"/>
+      <c r="N30" s="0"/>
+      <c r="O30" s="0"/>
+      <c r="P30" s="0"/>
+      <c r="Q30" s="0"/>
+      <c r="R30" s="0"/>
+      <c r="S30" s="0"/>
       <c r="T30" s="0"/>
+      <c r="U30" s="0"/>
+      <c r="V30" s="0"/>
+      <c r="W30" s="0"/>
+      <c r="X30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-      <c r="P31" s="3"/>
-      <c r="R31" s="3"/>
+      <c r="D31" s="0"/>
+      <c r="E31" s="0"/>
+      <c r="F31" s="0"/>
+      <c r="G31" s="0"/>
+      <c r="H31" s="0"/>
+      <c r="I31" s="0"/>
+      <c r="J31" s="0"/>
+      <c r="K31" s="0"/>
+      <c r="L31" s="0"/>
+      <c r="M31" s="0"/>
+      <c r="N31" s="0"/>
+      <c r="O31" s="0"/>
+      <c r="P31" s="0"/>
+      <c r="Q31" s="0"/>
+      <c r="R31" s="0"/>
+      <c r="S31" s="0"/>
       <c r="T31" s="0"/>
+      <c r="U31" s="0"/>
+      <c r="V31" s="0"/>
+      <c r="W31" s="0"/>
+      <c r="X31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="M32" s="3"/>
-      <c r="N32" s="3"/>
-      <c r="O32" s="3"/>
-      <c r="P32" s="3"/>
-      <c r="R32" s="3"/>
+      <c r="D32" s="0"/>
+      <c r="E32" s="0"/>
+      <c r="F32" s="0"/>
+      <c r="G32" s="0"/>
+      <c r="H32" s="0"/>
+      <c r="I32" s="0"/>
+      <c r="J32" s="0"/>
+      <c r="K32" s="0"/>
+      <c r="L32" s="0"/>
+      <c r="M32" s="0"/>
+      <c r="N32" s="0"/>
+      <c r="O32" s="0"/>
+      <c r="P32" s="0"/>
+      <c r="Q32" s="0"/>
+      <c r="R32" s="0"/>
+      <c r="S32" s="0"/>
       <c r="T32" s="0"/>
+      <c r="U32" s="0"/>
+      <c r="V32" s="0"/>
+      <c r="W32" s="0"/>
+      <c r="X32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="N33" s="3"/>
-      <c r="O33" s="3"/>
-      <c r="P33" s="3"/>
-      <c r="R33" s="3"/>
+      <c r="D33" s="0"/>
+      <c r="E33" s="0"/>
+      <c r="F33" s="0"/>
+      <c r="G33" s="0"/>
+      <c r="H33" s="0"/>
+      <c r="I33" s="0"/>
+      <c r="J33" s="0"/>
+      <c r="K33" s="0"/>
+      <c r="L33" s="0"/>
+      <c r="M33" s="0"/>
+      <c r="N33" s="0"/>
+      <c r="O33" s="0"/>
+      <c r="P33" s="0"/>
+      <c r="Q33" s="0"/>
+      <c r="R33" s="0"/>
+      <c r="S33" s="0"/>
       <c r="T33" s="0"/>
+      <c r="U33" s="0"/>
+      <c r="V33" s="0"/>
+      <c r="W33" s="0"/>
+      <c r="X33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="K34" s="3"/>
-      <c r="M34" s="3"/>
-      <c r="N34" s="3"/>
-      <c r="P34" s="3"/>
-      <c r="R34" s="3"/>
-      <c r="S34" s="3"/>
+      <c r="D34" s="0"/>
+      <c r="E34" s="0"/>
+      <c r="F34" s="0"/>
+      <c r="G34" s="0"/>
+      <c r="H34" s="0"/>
+      <c r="I34" s="0"/>
+      <c r="J34" s="0"/>
+      <c r="K34" s="0"/>
+      <c r="L34" s="0"/>
+      <c r="M34" s="0"/>
+      <c r="N34" s="0"/>
+      <c r="O34" s="0"/>
+      <c r="P34" s="0"/>
+      <c r="Q34" s="0"/>
+      <c r="R34" s="0"/>
+      <c r="S34" s="0"/>
       <c r="T34" s="0"/>
+      <c r="U34" s="0"/>
+      <c r="V34" s="0"/>
+      <c r="W34" s="0"/>
+      <c r="X34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="3"/>

</xml_diff>